<commit_message>
added Name to metadata file for contributor (ORCID not enough for published doi)
New version 3. - draft - write back DOI to xls after minting
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://anu365-my.sharepoint.com/personal/u1173285_anu_edu_au/Documents/Documents/datacite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{5B25795F-DB20-8F42-9C52-534693E9D665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26F13AB2-0D44-CC44-996F-4BC0866E83D2}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{5B25795F-DB20-8F42-9C52-534693E9D665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{849483DB-6E8E-AC41-8A8E-65915AC36600}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="1480" windowWidth="23820" windowHeight="16820" xr2:uid="{E48FA8C3-F92E-AE41-9EBA-19F2ECD8ACF3}"/>
+    <workbookView xWindow="37860" yWindow="2420" windowWidth="36260" windowHeight="16820" xr2:uid="{E48FA8C3-F92E-AE41-9EBA-19F2ECD8ACF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>title</t>
   </si>
@@ -80,14 +80,20 @@
     <t>https://orcid.org/0000-0001-7475-4487</t>
   </si>
   <si>
-    <t>Wednesday 1030</t>
+    <t>fresh123</t>
+  </si>
+  <si>
+    <t>Contrib_name</t>
+  </si>
+  <si>
+    <t>Rossow, Nick</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,6 +105,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -264,8 +276,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DFA3099-4C90-2A4C-80E6-ED499DCD9E69}" name="Table1" displayName="Table1" ref="E1:I2" totalsRowShown="0">
-  <autoFilter ref="E1:I2" xr:uid="{7DFA3099-4C90-2A4C-80E6-ED499DCD9E69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DFA3099-4C90-2A4C-80E6-ED499DCD9E69}" name="Table1" displayName="Table1" ref="F1:J2" totalsRowShown="0">
+  <autoFilter ref="F1:J2" xr:uid="{7DFA3099-4C90-2A4C-80E6-ED499DCD9E69}"/>
   <tableColumns count="5">
     <tableColumn id="3" xr3:uid="{749D3F4B-A4EA-5947-8084-B1D1104FA5E5}" name="Pub_ROR" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{CBAC6362-3B40-1A45-BC6B-8C23403AB08B}" name="url" dataDxfId="3"/>
@@ -594,22 +606,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CDE64C-09E6-0145-A1D4-5C5C1C827E27}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" customWidth="1"/>
-    <col min="6" max="6" width="37.83203125" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="37.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -623,22 +638,25 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -651,23 +669,41 @@
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F3" s="1"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F4" s="1"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{5D3E0D90-3723-F347-8AED-B8A1CB2D1101}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{5D3E0D90-3723-F347-8AED-B8A1CB2D1101}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>